<commit_message>
Updated with f2_ocr_formatter fixes and f3_ocr_formatter integration
</commit_message>
<xml_diff>
--- a/parameters/no_of_vars.xlsx
+++ b/parameters/no_of_vars.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="form1" sheetId="3" r:id="rId1"/>
@@ -164,7 +164,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +172,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +189,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -199,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -210,6 +240,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2867,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2891,7 +2926,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2902,7 +2937,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2913,7 +2948,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <v>4</v>
       </c>
     </row>
@@ -2924,7 +2959,7 @@
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <v>6</v>
       </c>
     </row>
@@ -2935,7 +2970,7 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="11">
         <v>0</v>
       </c>
     </row>
@@ -2946,7 +2981,7 @@
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="10">
         <v>2</v>
       </c>
     </row>
@@ -2957,7 +2992,7 @@
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="13">
         <v>2</v>
       </c>
     </row>
@@ -2968,7 +3003,7 @@
       <c r="B9">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="13">
         <v>2</v>
       </c>
     </row>
@@ -2979,7 +3014,7 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <v>2</v>
       </c>
     </row>
@@ -2990,7 +3025,7 @@
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3001,7 +3036,7 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="13">
         <v>2</v>
       </c>
     </row>
@@ -3012,7 +3047,7 @@
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3023,7 +3058,7 @@
       <c r="B14">
         <v>3</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3034,7 +3069,7 @@
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3045,7 +3080,7 @@
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3056,7 +3091,7 @@
       <c r="B17">
         <v>3</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="12">
         <v>2</v>
       </c>
     </row>
@@ -3067,7 +3102,7 @@
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3078,7 +3113,7 @@
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3089,7 +3124,7 @@
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="12">
         <v>2</v>
       </c>
     </row>
@@ -3100,7 +3135,7 @@
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3111,7 +3146,7 @@
       <c r="B22">
         <v>3</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="12">
         <v>2</v>
       </c>
     </row>
@@ -3122,7 +3157,7 @@
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="12">
         <v>2</v>
       </c>
     </row>
@@ -3133,7 +3168,7 @@
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3144,7 +3179,7 @@
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="10">
         <v>0</v>
       </c>
     </row>
@@ -3155,7 +3190,7 @@
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3166,7 +3201,7 @@
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="10">
         <v>2</v>
       </c>
     </row>
@@ -3177,7 +3212,7 @@
       <c r="B28">
         <v>2</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="14">
         <v>2</v>
       </c>
     </row>
@@ -3188,7 +3223,7 @@
       <c r="B29">
         <v>2</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="14">
         <v>4</v>
       </c>
     </row>
@@ -3370,8 +3405,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <customProperties>
-    <customPr name="OrphanNamesChecked" r:id="rId1"/>
+    <customPr name="OrphanNamesChecked" r:id="rId2"/>
   </customProperties>
 </worksheet>
 </file>
</xml_diff>